<commit_message>
Update release version to 1.0.0 in documentation
</commit_message>
<xml_diff>
--- a/DeveloperGuide/SPARQL/Performance/dotNetRDF BSBM v3 Benchmark.xlsx
+++ b/DeveloperGuide/SPARQL/Performance/dotNetRDF BSBM v3 Benchmark.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="24675" windowHeight="10515" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="340" windowWidth="35660" windowHeight="17280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="In-Memory Results" sheetId="1" r:id="rId1"/>
     <sheet name="In-Memory Comparisons" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
   <si>
     <t>Test Data</t>
   </si>
@@ -106,12 +111,18 @@
   <si>
     <t>Leviathan 0.8.1</t>
   </si>
+  <si>
+    <t>Leviathan 1.0.0</t>
+  </si>
+  <si>
+    <t>Leviathan 0.8.1 - These results are suspect because a bug in the config meant they didn't actually query any data (oops)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,13 +162,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -170,16 +203,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -188,15 +221,23 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -231,20 +272,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -260,7 +329,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -325,34 +394,34 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4991</c:v>
+                  <c:v>4991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22716</c:v>
+                  <c:v>22716.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40333</c:v>
+                  <c:v>40333.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98113</c:v>
+                  <c:v>98113.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>191502</c:v>
+                  <c:v>191502.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375114</c:v>
+                  <c:v>375114.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>550078</c:v>
+                  <c:v>550078.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>725515</c:v>
+                  <c:v>725515.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900517</c:v>
+                  <c:v>900517.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000313</c:v>
+                  <c:v>1.000313E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -373,25 +442,25 @@
                   <c:v>16.241</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.239000000000001</c:v>
+                  <c:v>27.239</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.332000000000001</c:v>
+                  <c:v>38.332</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54.933999999999997</c:v>
+                  <c:v>54.934</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>125.60299999999999</c:v>
+                  <c:v>125.603</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>204.999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>302.77600000000001</c:v>
+                  <c:v>302.776</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>370.24099999999999</c:v>
+                  <c:v>370.241</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -422,34 +491,34 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4991</c:v>
+                  <c:v>4991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22716</c:v>
+                  <c:v>22716.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40333</c:v>
+                  <c:v>40333.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98113</c:v>
+                  <c:v>98113.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>191502</c:v>
+                  <c:v>191502.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375114</c:v>
+                  <c:v>375114.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>550078</c:v>
+                  <c:v>550078.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>725515</c:v>
+                  <c:v>725515.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900517</c:v>
+                  <c:v>900517.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000313</c:v>
+                  <c:v>1.000313E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,13 +530,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9.6150000000000002</c:v>
+                  <c:v>9.615</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10.14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.933999999999999</c:v>
+                  <c:v>10.934</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>14.315</c:v>
@@ -479,7 +548,7 @@
                   <c:v>15.843</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.623000000000001</c:v>
+                  <c:v>19.623</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>22.558</c:v>
@@ -488,7 +557,7 @@
                   <c:v>26.253</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26.946999999999999</c:v>
+                  <c:v>26.947</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -496,18 +565,10 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="3"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'In-Memory Comparisons'!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Leviathan 0.8.1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Leviathan 1.0.0</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -519,73 +580,64 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4991</c:v>
+                  <c:v>4991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22716</c:v>
+                  <c:v>22716.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40333</c:v>
+                  <c:v>40333.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98113</c:v>
+                  <c:v>98113.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>191502</c:v>
+                  <c:v>191502.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375114</c:v>
+                  <c:v>375114.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>550078</c:v>
+                  <c:v>550078.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>725515</c:v>
+                  <c:v>725515.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900517</c:v>
+                  <c:v>900517.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000313</c:v>
+                  <c:v>1.000313E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'In-Memory Comparisons'!$B$5:$K$5</c:f>
+              <c:f>'In-Memory Comparisons'!$B$6:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7.0030000000000001</c:v>
+                  <c:v>7.187</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.3289999999999997</c:v>
+                  <c:v>7.634</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9720000000000004</c:v>
+                  <c:v>7.491</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.0339999999999998</c:v>
+                  <c:v>8.507</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.9960000000000004</c:v>
+                  <c:v>9.254</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0140000000000002</c:v>
+                  <c:v>9.395</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.1660000000000004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.1929999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.1719999999999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7.2060000000000004</c:v>
+                  <c:v>11.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -600,11 +652,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="100319808"/>
-        <c:axId val="100320384"/>
+        <c:axId val="2087536024"/>
+        <c:axId val="2124328248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100319808"/>
+        <c:axId val="2087536024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -637,12 +689,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100320384"/>
+        <c:crossAx val="2124328248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100320384"/>
+        <c:axId val="2124328248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -677,7 +729,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100319808"/>
+        <c:crossAx val="2087536024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -702,7 +754,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -748,7 +800,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'In-Memory Comparisons'!$A$9</c:f>
+              <c:f>'In-Memory Comparisons'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -762,46 +814,46 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'In-Memory Comparisons'!$B$8:$K$8</c:f>
+              <c:f>'In-Memory Comparisons'!$B$9:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4991</c:v>
+                  <c:v>4991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22716</c:v>
+                  <c:v>22716.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40333</c:v>
+                  <c:v>40333.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98113</c:v>
+                  <c:v>98113.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>191502</c:v>
+                  <c:v>191502.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375114</c:v>
+                  <c:v>375114.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>550078</c:v>
+                  <c:v>550078.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>725515</c:v>
+                  <c:v>725515.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900517</c:v>
+                  <c:v>900517.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000313</c:v>
+                  <c:v>1.000313E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'In-Memory Comparisons'!$B$9:$K$9</c:f>
+              <c:f>'In-Memory Comparisons'!$B$10:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -845,7 +897,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'In-Memory Comparisons'!$A$10</c:f>
+              <c:f>'In-Memory Comparisons'!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -859,136 +911,39 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'In-Memory Comparisons'!$B$8:$K$8</c:f>
+              <c:f>'In-Memory Comparisons'!$B$9:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4991</c:v>
+                  <c:v>4991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22716</c:v>
+                  <c:v>22716.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40333</c:v>
+                  <c:v>40333.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98113</c:v>
+                  <c:v>98113.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>191502</c:v>
+                  <c:v>191502.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375114</c:v>
+                  <c:v>375114.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>550078</c:v>
+                  <c:v>550078.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>725515</c:v>
+                  <c:v>725515.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900517</c:v>
+                  <c:v>900517.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000313</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'In-Memory Comparisons'!$B$10:$K$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>18721.009999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17751.37</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16463.080000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12573.83</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10361.57</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11361.44</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9172.9500000000007</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7979.48</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6856.41</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6679.68</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'In-Memory Comparisons'!$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Leviathan 0.8.1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'In-Memory Comparisons'!$B$8:$K$8</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>4991</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>22716</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>98113</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>191502</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>375114</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>550078</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>725515</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>900517</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1000313</c:v>
+                  <c:v>1.000313E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1000,34 +955,114 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>25702.85</c:v>
+                  <c:v>18721.01</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24558.92</c:v>
+                  <c:v>17751.37</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25817.48</c:v>
+                  <c:v>16463.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25588.799999999999</c:v>
+                  <c:v>12573.83</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25730.69</c:v>
+                  <c:v>10361.57</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25662.14</c:v>
+                  <c:v>11361.44</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25117.74</c:v>
+                  <c:v>9172.950000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25024.71</c:v>
+                  <c:v>7979.48</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25097.41</c:v>
+                  <c:v>6856.41</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24978.46</c:v>
+                  <c:v>6679.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Leviathan 1.0.0</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'In-Memory Comparisons'!$B$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4991.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22716.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40333.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98113.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>191502.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375114.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550078.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>725515.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900517.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.000313E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'In-Memory Comparisons'!$B$13:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>25046.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23578.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24029.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21158.17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19451.38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19158.49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16043.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1042,11 +1077,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="58766400"/>
-        <c:axId val="58766976"/>
+        <c:axId val="2087562104"/>
+        <c:axId val="2087567624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58766400"/>
+        <c:axId val="2087562104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,12 +1110,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58766976"/>
+        <c:crossAx val="2087567624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58766976"/>
+        <c:axId val="2087567624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,8 +1142,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.5942028985507246E-2"/>
-              <c:y val="0.2250395731957554"/>
+              <c:x val="0.0159420289855072"/>
+              <c:y val="0.225039573195755"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1117,7 +1152,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58766400"/>
+        <c:crossAx val="2087562104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1142,7 +1177,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1207,34 +1242,34 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4991</c:v>
+                  <c:v>4991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22716</c:v>
+                  <c:v>22716.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40333</c:v>
+                  <c:v>40333.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98113</c:v>
+                  <c:v>98113.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>191502</c:v>
+                  <c:v>191502.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375114</c:v>
+                  <c:v>375114.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>550078</c:v>
+                  <c:v>550078.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>725515</c:v>
+                  <c:v>725515.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900517</c:v>
+                  <c:v>900517.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000313</c:v>
+                  <c:v>1.000313E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1246,13 +1281,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9.6150000000000002</c:v>
+                  <c:v>9.615</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10.14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.933999999999999</c:v>
+                  <c:v>10.934</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>14.315</c:v>
@@ -1264,7 +1299,7 @@
                   <c:v>15.843</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.623000000000001</c:v>
+                  <c:v>19.623</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>22.558</c:v>
@@ -1273,7 +1308,7 @@
                   <c:v>26.253</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26.946999999999999</c:v>
+                  <c:v>26.947</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1281,18 +1316,10 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'In-Memory Comparisons'!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Leviathan 0.8.1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Leviathan 1.0.0</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -1304,73 +1331,64 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4991</c:v>
+                  <c:v>4991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22716</c:v>
+                  <c:v>22716.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40333</c:v>
+                  <c:v>40333.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98113</c:v>
+                  <c:v>98113.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>191502</c:v>
+                  <c:v>191502.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375114</c:v>
+                  <c:v>375114.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>550078</c:v>
+                  <c:v>550078.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>725515</c:v>
+                  <c:v>725515.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900517</c:v>
+                  <c:v>900517.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000313</c:v>
+                  <c:v>1.000313E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'In-Memory Comparisons'!$B$5:$K$5</c:f>
+              <c:f>'In-Memory Comparisons'!$B$6:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7.0030000000000001</c:v>
+                  <c:v>7.187</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.3289999999999997</c:v>
+                  <c:v>7.634</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9720000000000004</c:v>
+                  <c:v>7.491</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.0339999999999998</c:v>
+                  <c:v>8.507</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.9960000000000004</c:v>
+                  <c:v>9.254</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0140000000000002</c:v>
+                  <c:v>9.395</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.1660000000000004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.1929999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.1719999999999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7.2060000000000004</c:v>
+                  <c:v>11.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1385,11 +1403,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="46714240"/>
-        <c:axId val="100322688"/>
+        <c:axId val="2087600824"/>
+        <c:axId val="2087606376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46714240"/>
+        <c:axId val="2087600824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,12 +1440,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100322688"/>
+        <c:crossAx val="2087606376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100322688"/>
+        <c:axId val="2087606376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1462,7 +1480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46714240"/>
+        <c:crossAx val="2087600824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1496,7 +1514,7 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1520,13 +1538,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>104776</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>333376</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1556,7 +1574,7 @@
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>52388</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1868,54 +1886,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36:I37"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39:I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" ht="18">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-    </row>
-    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" ht="18">
       <c r="A2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:11" ht="15">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1950,22 +1968,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:11">
+      <c r="A5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="5">
         <v>10</v>
       </c>
@@ -2000,7 +2018,7 @@
         <v>0.25258999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="5">
         <v>50</v>
       </c>
@@ -2035,7 +2053,7 @@
         <v>0.25997999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="5">
         <v>100</v>
       </c>
@@ -2070,7 +2088,7 @@
         <v>0.32089000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="5">
         <v>250</v>
       </c>
@@ -2105,7 +2123,7 @@
         <v>0.53708999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="5">
         <v>500</v>
       </c>
@@ -2140,7 +2158,7 @@
         <v>0.74114999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="5">
         <v>1000</v>
       </c>
@@ -2175,7 +2193,7 @@
         <v>0.99868999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="8">
         <v>1500</v>
       </c>
@@ -2210,7 +2228,7 @@
         <v>2.16133</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="8">
         <v>2000</v>
       </c>
@@ -2245,7 +2263,7 @@
         <v>3.5819200000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="8">
         <v>2500</v>
       </c>
@@ -2280,7 +2298,7 @@
         <v>5.2458799999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="11">
         <v>2785</v>
       </c>
@@ -2315,22 +2333,22 @@
         <v>6.5285500000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:11">
+      <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="5">
         <v>10</v>
       </c>
@@ -2365,7 +2383,7 @@
         <v>0.19173999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="5">
         <v>50</v>
       </c>
@@ -2400,7 +2418,7 @@
         <v>0.2021</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="5">
         <v>100</v>
       </c>
@@ -2435,7 +2453,7 @@
         <v>0.21823999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="5">
         <v>250</v>
       </c>
@@ -2470,7 +2488,7 @@
         <v>0.27937000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="5">
         <v>500</v>
       </c>
@@ -2505,7 +2523,7 @@
         <v>0.34117999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="5">
         <v>1000</v>
       </c>
@@ -2540,7 +2558,7 @@
         <v>0.31319000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="8">
         <v>1500</v>
       </c>
@@ -2575,7 +2593,7 @@
         <v>0.38673000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="8">
         <v>2000</v>
       </c>
@@ -2610,7 +2628,7 @@
         <v>0.44183</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="8">
         <v>2500</v>
       </c>
@@ -2645,7 +2663,7 @@
         <v>0.51507000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="11">
         <v>2785</v>
       </c>
@@ -2680,373 +2698,703 @@
         <v>0.53037000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>10</v>
-      </c>
-      <c r="B28" s="6">
+    <row r="27" spans="1:11">
+      <c r="A27" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="19">
+        <v>10</v>
+      </c>
+      <c r="B28" s="20">
         <v>4991</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="5">
-        <v>10</v>
-      </c>
-      <c r="E28" s="5">
-        <v>50</v>
-      </c>
-      <c r="F28" s="10">
+      <c r="D28" s="19">
+        <v>10</v>
+      </c>
+      <c r="E28" s="19">
+        <v>50</v>
+      </c>
+      <c r="F28" s="22">
         <v>0.13089999999999999</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="22">
         <v>0.20019999999999999</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28" s="22">
         <v>7.0030000000000001</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="22">
         <v>25702.85</v>
       </c>
-      <c r="J28" s="10">
+      <c r="J28" s="22">
         <v>0.14005999999999999</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="22">
         <v>0.13971</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>50</v>
-      </c>
-      <c r="B29" s="6">
+    <row r="29" spans="1:11">
+      <c r="A29" s="19">
+        <v>50</v>
+      </c>
+      <c r="B29" s="20">
         <v>22716</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="5">
-        <v>10</v>
-      </c>
-      <c r="E29" s="5">
-        <v>50</v>
-      </c>
-      <c r="F29" s="10">
+      <c r="D29" s="19">
+        <v>10</v>
+      </c>
+      <c r="E29" s="19">
+        <v>50</v>
+      </c>
+      <c r="F29" s="22">
         <v>0.1305</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="22">
         <v>0.1822</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="22">
         <v>7.3289999999999997</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="22">
         <v>24558.92</v>
       </c>
-      <c r="J29" s="10">
+      <c r="J29" s="22">
         <v>0.14659</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="22">
         <v>0.14616000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+    <row r="30" spans="1:11">
+      <c r="A30" s="19">
         <v>100</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="20">
         <v>40333</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="5">
-        <v>10</v>
-      </c>
-      <c r="E30" s="5">
-        <v>50</v>
-      </c>
-      <c r="F30" s="10">
+      <c r="D30" s="19">
+        <v>10</v>
+      </c>
+      <c r="E30" s="19">
+        <v>50</v>
+      </c>
+      <c r="F30" s="22">
         <v>0.13100000000000001</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="22">
         <v>0.15559999999999999</v>
       </c>
-      <c r="H30" s="10">
+      <c r="H30" s="22">
         <v>6.9720000000000004</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I30" s="22">
         <v>25817.48</v>
       </c>
-      <c r="J30" s="10">
+      <c r="J30" s="22">
         <v>0.13944000000000001</v>
       </c>
-      <c r="K30" s="10">
+      <c r="K30" s="22">
         <v>0.13932</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+    <row r="31" spans="1:11">
+      <c r="A31" s="19">
         <v>250</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="20">
         <v>98113</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="5">
-        <v>10</v>
-      </c>
-      <c r="E31" s="5">
-        <v>50</v>
-      </c>
-      <c r="F31" s="10">
+      <c r="D31" s="19">
+        <v>10</v>
+      </c>
+      <c r="E31" s="19">
+        <v>50</v>
+      </c>
+      <c r="F31" s="22">
         <v>0.12820000000000001</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G31" s="22">
         <v>0.20569999999999999</v>
       </c>
-      <c r="H31" s="10">
+      <c r="H31" s="22">
         <v>7.0339999999999998</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="22">
         <v>25588.799999999999</v>
       </c>
-      <c r="J31" s="10">
+      <c r="J31" s="22">
         <v>0.14069000000000001</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K31" s="22">
         <v>0.14027999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+    <row r="32" spans="1:11">
+      <c r="A32" s="19">
         <v>500</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="20">
         <v>191502</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="5">
-        <v>10</v>
-      </c>
-      <c r="E32" s="5">
-        <v>50</v>
-      </c>
-      <c r="F32" s="10">
+      <c r="D32" s="19">
+        <v>10</v>
+      </c>
+      <c r="E32" s="19">
+        <v>50</v>
+      </c>
+      <c r="F32" s="22">
         <v>0.13089999999999999</v>
       </c>
-      <c r="G32" s="10">
+      <c r="G32" s="22">
         <v>0.15110000000000001</v>
       </c>
-      <c r="H32" s="10">
+      <c r="H32" s="22">
         <v>6.9960000000000004</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="22">
         <v>25730.69</v>
       </c>
-      <c r="J32" s="10">
+      <c r="J32" s="22">
         <v>0.13991000000000001</v>
       </c>
-      <c r="K32" s="10">
+      <c r="K32" s="22">
         <v>0.13980999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+    <row r="33" spans="1:11">
+      <c r="A33" s="19">
         <v>1000</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="20">
         <v>375114</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="5">
-        <v>10</v>
-      </c>
-      <c r="E33" s="5">
-        <v>50</v>
-      </c>
-      <c r="F33" s="10">
+      <c r="D33" s="19">
+        <v>10</v>
+      </c>
+      <c r="E33" s="19">
+        <v>50</v>
+      </c>
+      <c r="F33" s="22">
         <v>0.12590000000000001</v>
       </c>
-      <c r="G33" s="10">
+      <c r="G33" s="22">
         <v>0.2024</v>
       </c>
-      <c r="H33" s="10">
+      <c r="H33" s="22">
         <v>7.0140000000000002</v>
       </c>
-      <c r="I33" s="10">
+      <c r="I33" s="22">
         <v>25662.14</v>
       </c>
-      <c r="J33" s="10">
+      <c r="J33" s="22">
         <v>0.14027999999999999</v>
       </c>
-      <c r="K33" s="10">
+      <c r="K33" s="22">
         <v>0.13991000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
+    <row r="34" spans="1:11">
+      <c r="A34" s="23">
         <v>1500</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="24">
         <v>550078</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="5">
-        <v>10</v>
-      </c>
-      <c r="E34" s="5">
-        <v>50</v>
-      </c>
-      <c r="F34" s="10">
+      <c r="D34" s="19">
+        <v>10</v>
+      </c>
+      <c r="E34" s="19">
+        <v>50</v>
+      </c>
+      <c r="F34" s="22">
         <v>0.1333</v>
       </c>
-      <c r="G34" s="10">
+      <c r="G34" s="22">
         <v>0.1736</v>
       </c>
-      <c r="H34" s="10">
+      <c r="H34" s="22">
         <v>7.1660000000000004</v>
       </c>
-      <c r="I34" s="10">
+      <c r="I34" s="22">
         <v>25117.74</v>
       </c>
-      <c r="J34" s="10">
+      <c r="J34" s="22">
         <v>0.14332</v>
       </c>
-      <c r="K34" s="10">
+      <c r="K34" s="22">
         <v>0.1431</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+    <row r="35" spans="1:11">
+      <c r="A35" s="23">
         <v>2000</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="24">
         <v>725515</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="5">
-        <v>10</v>
-      </c>
-      <c r="E35" s="5">
-        <v>50</v>
-      </c>
-      <c r="F35" s="10">
+      <c r="D35" s="19">
+        <v>10</v>
+      </c>
+      <c r="E35" s="19">
+        <v>50</v>
+      </c>
+      <c r="F35" s="22">
         <v>0.1298</v>
       </c>
-      <c r="G35" s="10">
+      <c r="G35" s="22">
         <v>0.26879999999999998</v>
       </c>
-      <c r="H35" s="10">
+      <c r="H35" s="22">
         <v>7.1929999999999996</v>
       </c>
-      <c r="I35" s="10">
+      <c r="I35" s="22">
         <v>25024.71</v>
       </c>
-      <c r="J35" s="10">
+      <c r="J35" s="22">
         <v>0.14385999999999999</v>
       </c>
-      <c r="K35" s="10">
+      <c r="K35" s="22">
         <v>0.1429</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+    <row r="36" spans="1:11">
+      <c r="A36" s="23">
         <v>2500</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="24">
         <v>900517</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="5">
-        <v>10</v>
-      </c>
-      <c r="E36" s="5">
-        <v>50</v>
-      </c>
-      <c r="F36" s="10">
+      <c r="D36" s="19">
+        <v>10</v>
+      </c>
+      <c r="E36" s="19">
+        <v>50</v>
+      </c>
+      <c r="F36" s="22">
         <v>0.1265</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="22">
         <v>0.29649999999999999</v>
       </c>
-      <c r="H36" s="10">
+      <c r="H36" s="22">
         <v>7.1719999999999997</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I36" s="22">
         <v>25097.41</v>
       </c>
-      <c r="J36" s="10">
+      <c r="J36" s="22">
         <v>0.14344000000000001</v>
       </c>
-      <c r="K36" s="10">
+      <c r="K36" s="22">
         <v>0.14201</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+    <row r="37" spans="1:11">
+      <c r="A37" s="23">
         <v>2785</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="24">
         <v>1000313</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="13">
-        <v>10</v>
-      </c>
-      <c r="E37" s="13">
-        <v>50</v>
-      </c>
-      <c r="F37" s="10">
+      <c r="D37" s="19">
+        <v>10</v>
+      </c>
+      <c r="E37" s="19">
+        <v>50</v>
+      </c>
+      <c r="F37" s="22">
         <v>0.13270000000000001</v>
       </c>
-      <c r="G37" s="10">
+      <c r="G37" s="22">
         <v>0.16259999999999999</v>
       </c>
-      <c r="H37" s="10">
+      <c r="H37" s="22">
         <v>7.2060000000000004</v>
       </c>
-      <c r="I37" s="10">
+      <c r="I37" s="22">
         <v>24978.46</v>
       </c>
-      <c r="J37" s="10">
+      <c r="J37" s="22">
         <v>0.14412</v>
       </c>
-      <c r="K37" s="10">
+      <c r="K37" s="22">
         <v>0.14399999999999999</v>
       </c>
     </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="5">
+        <v>10</v>
+      </c>
+      <c r="B39" s="6">
+        <v>4991</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="5">
+        <v>10</v>
+      </c>
+      <c r="E39" s="5">
+        <v>50</v>
+      </c>
+      <c r="F39" s="10">
+        <v>0.11609999999999999</v>
+      </c>
+      <c r="G39" s="10">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="H39" s="10">
+        <v>7.1870000000000003</v>
+      </c>
+      <c r="I39" s="10">
+        <v>25046.5</v>
+      </c>
+      <c r="J39" s="10">
+        <v>0.14373</v>
+      </c>
+      <c r="K39" s="10">
+        <v>0.13639000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="5">
+        <v>50</v>
+      </c>
+      <c r="B40" s="6">
+        <v>22716</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="5">
+        <v>10</v>
+      </c>
+      <c r="E40" s="5">
+        <v>50</v>
+      </c>
+      <c r="F40" s="10">
+        <v>0.12559999999999999</v>
+      </c>
+      <c r="G40" s="10">
+        <v>0.68440000000000001</v>
+      </c>
+      <c r="H40" s="10">
+        <v>7.6340000000000003</v>
+      </c>
+      <c r="I40" s="10">
+        <v>23578.45</v>
+      </c>
+      <c r="J40" s="10">
+        <v>0.15268000000000001</v>
+      </c>
+      <c r="K40" s="10">
+        <v>0.14582000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="5">
+        <v>100</v>
+      </c>
+      <c r="B41" s="6">
+        <v>40333</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="5">
+        <v>10</v>
+      </c>
+      <c r="E41" s="5">
+        <v>50</v>
+      </c>
+      <c r="F41" s="10">
+        <v>0.12920000000000001</v>
+      </c>
+      <c r="G41" s="10">
+        <v>0.18640000000000001</v>
+      </c>
+      <c r="H41" s="10">
+        <v>7.4909999999999997</v>
+      </c>
+      <c r="I41" s="10">
+        <v>24029.33</v>
+      </c>
+      <c r="J41" s="10">
+        <v>0.14982000000000001</v>
+      </c>
+      <c r="K41" s="10">
+        <v>0.14927000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="5">
+        <v>250</v>
+      </c>
+      <c r="B42" s="6">
+        <v>98113</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="5">
+        <v>10</v>
+      </c>
+      <c r="E42" s="5">
+        <v>50</v>
+      </c>
+      <c r="F42" s="10">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="G42" s="10">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="H42" s="10">
+        <v>8.5069999999999997</v>
+      </c>
+      <c r="I42" s="10">
+        <v>21158.17</v>
+      </c>
+      <c r="J42" s="10">
+        <v>0.17015</v>
+      </c>
+      <c r="K42" s="10">
+        <v>0.16971</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="5">
+        <v>500</v>
+      </c>
+      <c r="B43" s="6">
+        <v>191502</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="5">
+        <v>10</v>
+      </c>
+      <c r="E43" s="5">
+        <v>50</v>
+      </c>
+      <c r="F43" s="10">
+        <v>0.15770000000000001</v>
+      </c>
+      <c r="G43" s="10">
+        <v>0.22869999999999999</v>
+      </c>
+      <c r="H43" s="10">
+        <v>9.2539999999999996</v>
+      </c>
+      <c r="I43" s="10">
+        <v>19451.38</v>
+      </c>
+      <c r="J43" s="10">
+        <v>0.18507999999999999</v>
+      </c>
+      <c r="K43" s="10">
+        <v>0.18445</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="5">
+        <v>1000</v>
+      </c>
+      <c r="B44" s="6">
+        <v>375114</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="5">
+        <v>10</v>
+      </c>
+      <c r="E44" s="5">
+        <v>50</v>
+      </c>
+      <c r="F44" s="10">
+        <v>0.1573</v>
+      </c>
+      <c r="G44" s="10">
+        <v>0.24279999999999999</v>
+      </c>
+      <c r="H44" s="10">
+        <v>9.3949999999999996</v>
+      </c>
+      <c r="I44" s="10">
+        <v>19158.490000000002</v>
+      </c>
+      <c r="J44" s="10">
+        <v>0.18790999999999999</v>
+      </c>
+      <c r="K44" s="10">
+        <v>0.187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="8">
+        <v>1500</v>
+      </c>
+      <c r="B45" s="9">
+        <v>550078</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="5">
+        <v>10</v>
+      </c>
+      <c r="E45" s="5">
+        <v>50</v>
+      </c>
+      <c r="F45" s="10">
+        <v>0.1799</v>
+      </c>
+      <c r="G45" s="10">
+        <v>0.2923</v>
+      </c>
+      <c r="H45" s="10">
+        <v>11.22</v>
+      </c>
+      <c r="I45" s="10">
+        <v>16043.17</v>
+      </c>
+      <c r="J45" s="10">
+        <v>0.22439000000000001</v>
+      </c>
+      <c r="K45" s="10">
+        <v>0.22309999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="8">
+        <v>2000</v>
+      </c>
+      <c r="B46" s="9">
+        <v>725515</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="5">
+        <v>10</v>
+      </c>
+      <c r="E46" s="5">
+        <v>50</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="8">
+        <v>2500</v>
+      </c>
+      <c r="B47" s="9">
+        <v>900517</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="5">
+        <v>10</v>
+      </c>
+      <c r="E47" s="5">
+        <v>50</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="11">
+        <v>2785</v>
+      </c>
+      <c r="B48" s="9">
+        <v>1000313</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="13">
+        <v>10</v>
+      </c>
+      <c r="E48" s="13">
+        <v>50</v>
+      </c>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A38:K38"/>
     <mergeCell ref="A16:K16"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A1:C1"/>
@@ -3056,24 +3404,29 @@
     <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="179" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="179" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" s="17" t="s">
         <v>27</v>
       </c>
@@ -3088,7 +3441,7 @@
       <c r="J1" s="17"/>
       <c r="K1" s="17"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" s="10"/>
       <c r="B2" s="6">
         <v>4991</v>
@@ -3121,7 +3474,7 @@
         <v>1000313</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
@@ -3156,7 +3509,7 @@
         <v>370.24099999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18">
       <c r="A4" s="10" t="s">
         <v>25</v>
       </c>
@@ -3191,205 +3544,268 @@
         <v>26.946999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:18">
+      <c r="A5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="22">
         <v>7.0030000000000001</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="22">
         <v>7.3289999999999997</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="22">
         <v>6.9720000000000004</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="22">
         <v>7.0339999999999998</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="22">
         <v>6.9960000000000004</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="22">
         <v>7.0140000000000002</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="22">
         <v>7.1660000000000004</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="22">
         <v>7.1929999999999996</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="22">
         <v>7.1719999999999997</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="22">
         <v>7.2060000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+    <row r="6" spans="1:18">
+      <c r="A6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="10">
+        <v>7.1870000000000003</v>
+      </c>
+      <c r="C6" s="10">
+        <v>7.6340000000000003</v>
+      </c>
+      <c r="D6" s="10">
+        <v>7.4909999999999997</v>
+      </c>
+      <c r="E6" s="10">
+        <v>8.5069999999999997</v>
+      </c>
+      <c r="F6" s="10">
+        <v>9.2539999999999996</v>
+      </c>
+      <c r="G6" s="10">
+        <v>9.3949999999999996</v>
+      </c>
+      <c r="H6" s="10">
+        <v>11.22</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="6">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="10"/>
+      <c r="B9" s="6">
         <v>4991</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C9" s="6">
         <v>22716</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="6">
         <v>40333</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E9" s="6">
         <v>98113</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F9" s="6">
         <v>191502</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G9" s="6">
         <v>375114</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H9" s="9">
         <v>550078</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I9" s="9">
         <v>725515</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J9" s="9">
         <v>900517</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K9" s="9">
         <v>1000313</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="10" spans="1:18">
+      <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B10" s="10">
         <v>13942.09</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C10" s="10">
         <v>13785.19</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D10" s="10">
         <v>11082.87</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E10" s="10">
         <v>6608.18</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F10" s="10">
         <v>4695.79</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G10" s="10">
         <v>3276.64</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H10" s="10">
         <v>1433.08</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I10" s="10">
         <v>878.05</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J10" s="10">
         <v>594.5</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K10" s="10">
         <v>486.17</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="11" spans="1:18">
+      <c r="A11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B11" s="10">
         <v>18721.009999999998</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C11" s="10">
         <v>17751.37</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D11" s="10">
         <v>16463.080000000002</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E11" s="10">
         <v>12573.83</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F11" s="10">
         <v>10361.57</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G11" s="10">
         <v>11361.44</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H11" s="10">
         <v>9172.9500000000007</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I11" s="10">
         <v>7979.48</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J11" s="10">
         <v>6856.41</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K11" s="10">
         <v>6679.68</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="12" spans="1:18">
+      <c r="A12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B12" s="22">
         <v>25702.85</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C12" s="22">
         <v>24558.92</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D12" s="22">
         <v>25817.48</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E12" s="22">
         <v>25588.799999999999</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F12" s="22">
         <v>25730.69</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G12" s="22">
         <v>25662.14</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H12" s="22">
         <v>25117.74</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I12" s="22">
         <v>25024.71</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J12" s="22">
         <v>25097.41</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K12" s="22">
         <v>24978.46</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="R15" t="s">
+    <row r="13" spans="1:18">
+      <c r="A13" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="10">
+        <v>25046.5</v>
+      </c>
+      <c r="C13" s="10">
+        <v>23578.45</v>
+      </c>
+      <c r="D13" s="10">
+        <v>24029.33</v>
+      </c>
+      <c r="E13" s="10">
+        <v>21158.17</v>
+      </c>
+      <c r="F13" s="10">
+        <v>19451.38</v>
+      </c>
+      <c r="G13" s="10">
+        <v>19158.490000000002</v>
+      </c>
+      <c r="H13" s="10">
+        <v>16043.17</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="R16" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>